<commit_message>
Typo fixes to classic keycap spreadsheet
</commit_message>
<xml_diff>
--- a/hardware/keyboard-classic/classic-ascii-keycaps.xlsx
+++ b/hardware/keyboard-classic/classic-ascii-keycaps.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dave/vsrc/unified_retro_keyboard/hardware/keyboard-classic/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A7C3764-26B4-BE43-AED0-143A7458676D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB34F5F8-E37A-6E4D-9902-102EE7F8EC93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19640" yWindow="5360" windowWidth="41160" windowHeight="30100" xr2:uid="{5947D8F6-B0FF-824B-90A6-066CA128251B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" refMode="R1C1"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="123">
   <si>
     <t>Size</t>
   </si>
@@ -402,18 +402,6 @@
   </si>
   <si>
     <t>Order specifications for Signature Plastics keycaps</t>
-  </si>
-  <si>
-    <t>TBT</t>
-  </si>
-  <si>
-    <t>??</t>
-  </si>
-  <si>
-    <t>YW</t>
-  </si>
-  <si>
-    <t>RUN</t>
   </si>
   <si>
     <t>Classic Keycap set</t>
@@ -459,7 +447,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -502,12 +490,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -536,13 +518,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>429346</xdr:colOff>
-      <xdr:row>87</xdr:row>
+      <xdr:row>84</xdr:row>
       <xdr:rowOff>118324</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>1795419</xdr:colOff>
-      <xdr:row>109</xdr:row>
+      <xdr:row>106</xdr:row>
       <xdr:rowOff>197206</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -879,10 +861,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D76B701B-B3BE-9240-9526-A5AC01D01246}">
-  <dimension ref="A1:K89"/>
+  <dimension ref="A1:K86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="161" zoomScaleNormal="161" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+    <sheetView tabSelected="1" zoomScale="161" zoomScaleNormal="161" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -900,20 +882,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A1" s="16" t="s">
-        <v>126</v>
-      </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="17" t="s">
+      <c r="A1" s="14" t="s">
+        <v>122</v>
+      </c>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="15" t="s">
         <v>99</v>
       </c>
-      <c r="F1" s="17"/>
-      <c r="G1" s="18">
-        <v>44505</v>
-      </c>
-      <c r="H1" s="16"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="16">
+        <v>44529</v>
+      </c>
+      <c r="H1" s="14"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="11"/>
@@ -1021,10 +1003,10 @@
         <v>1</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>122</v>
+        <v>102</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>4</v>
@@ -1039,22 +1021,25 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
-        <f t="shared" ref="A11:A77" si="0">A10+1</f>
+        <f t="shared" ref="A11:A75" si="0">A10+1</f>
         <v>2</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>124</v>
+        <v>102</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>112</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="I11" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="J11" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="K11" s="14"/>
+      <c r="G11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="J11" s="1"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
@@ -1071,7 +1056,7 @@
         <v>4</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H12" s="1" t="s">
         <v>105</v>
@@ -1093,7 +1078,7 @@
         <v>4</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H13" s="1" t="s">
         <v>105</v>
@@ -1115,7 +1100,7 @@
         <v>4</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H14" s="1" t="s">
         <v>105</v>
@@ -1137,17 +1122,20 @@
         <v>4</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H15" s="1" t="s">
         <v>105</v>
       </c>
       <c r="J15" s="1"/>
+      <c r="K15" s="6" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
-        <f>A14+1</f>
-        <v>6</v>
+        <f t="shared" si="0"/>
+        <v>7</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>102</v>
@@ -1158,19 +1146,24 @@
       <c r="D16" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="E16" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>53</v>
+      </c>
       <c r="G16" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H16" s="1" t="s">
         <v>105</v>
       </c>
       <c r="J16" s="1"/>
-      <c r="K16" s="15"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
-        <f>A15+1</f>
-        <v>7</v>
+        <f t="shared" si="0"/>
+        <v>8</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>102</v>
@@ -1182,20 +1175,17 @@
         <v>4</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H17" s="1" t="s">
         <v>105</v>
       </c>
       <c r="J17" s="1"/>
-      <c r="K17" s="6" t="s">
-        <v>98</v>
-      </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>102</v>
@@ -1206,14 +1196,8 @@
       <c r="D18" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E18" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>53</v>
-      </c>
       <c r="G18" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H18" s="1" t="s">
         <v>105</v>
@@ -1223,7 +1207,7 @@
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>102</v>
@@ -1235,7 +1219,7 @@
         <v>4</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="H19" s="1" t="s">
         <v>105</v>
@@ -1245,7 +1229,7 @@
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>102</v>
@@ -1257,17 +1241,20 @@
         <v>4</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="H20" s="1" t="s">
         <v>105</v>
       </c>
       <c r="J20" s="1"/>
+      <c r="K20" s="6" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>102</v>
@@ -1279,7 +1266,7 @@
         <v>4</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="H21" s="1" t="s">
         <v>105</v>
@@ -1289,7 +1276,7 @@
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>102</v>
@@ -1301,7 +1288,7 @@
         <v>4</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="H22" s="1" t="s">
         <v>105</v>
@@ -1311,7 +1298,7 @@
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <f t="shared" si="0"/>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>102</v>
@@ -1323,20 +1310,17 @@
         <v>4</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="H23" s="1" t="s">
         <v>105</v>
       </c>
       <c r="J23" s="1"/>
-      <c r="K23" s="6" t="s">
-        <v>98</v>
-      </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>102</v>
@@ -1348,7 +1332,7 @@
         <v>4</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="H24" s="1" t="s">
         <v>105</v>
@@ -1358,7 +1342,7 @@
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>102</v>
@@ -1369,8 +1353,14 @@
       <c r="D25" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="E25" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>105</v>
+      </c>
       <c r="G25" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="H25" s="1" t="s">
         <v>105</v>
@@ -1380,7 +1370,7 @@
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>102</v>
@@ -1392,7 +1382,7 @@
         <v>4</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="H26" s="1" t="s">
         <v>105</v>
@@ -1402,7 +1392,7 @@
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <f t="shared" si="0"/>
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>102</v>
@@ -1414,7 +1404,7 @@
         <v>4</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="H27" s="1" t="s">
         <v>105</v>
@@ -1424,7 +1414,7 @@
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <f t="shared" si="0"/>
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>102</v>
@@ -1436,13 +1426,13 @@
         <v>4</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F28" s="1" t="s">
         <v>105</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="H28" s="1" t="s">
         <v>105</v>
@@ -1452,7 +1442,7 @@
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>102</v>
@@ -1464,7 +1454,7 @@
         <v>4</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="H29" s="1" t="s">
         <v>105</v>
@@ -1474,7 +1464,7 @@
     <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>102</v>
@@ -1486,7 +1476,7 @@
         <v>4</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="H30" s="1" t="s">
         <v>105</v>
@@ -1496,7 +1486,7 @@
     <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <f t="shared" si="0"/>
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>102</v>
@@ -1507,14 +1497,8 @@
       <c r="D31" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E31" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>105</v>
-      </c>
       <c r="G31" s="1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="H31" s="1" t="s">
         <v>105</v>
@@ -1524,7 +1508,7 @@
     <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <f t="shared" si="0"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>102</v>
@@ -1536,7 +1520,7 @@
         <v>4</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="H32" s="1" t="s">
         <v>105</v>
@@ -1546,7 +1530,7 @@
     <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <f t="shared" si="0"/>
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>102</v>
@@ -1558,7 +1542,7 @@
         <v>4</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="H33" s="1" t="s">
         <v>105</v>
@@ -1568,7 +1552,7 @@
     <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <f t="shared" si="0"/>
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>102</v>
@@ -1580,7 +1564,7 @@
         <v>4</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="H34" s="1" t="s">
         <v>105</v>
@@ -1590,7 +1574,7 @@
     <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <f t="shared" si="0"/>
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>102</v>
@@ -1602,7 +1586,7 @@
         <v>4</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="H35" s="1" t="s">
         <v>105</v>
@@ -1612,7 +1596,7 @@
     <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <f t="shared" si="0"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>102</v>
@@ -1624,7 +1608,7 @@
         <v>4</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H36" s="1" t="s">
         <v>105</v>
@@ -1634,7 +1618,7 @@
     <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <f t="shared" si="0"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>102</v>
@@ -1646,7 +1630,7 @@
         <v>4</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="H37" s="1" t="s">
         <v>105</v>
@@ -1656,7 +1640,7 @@
     <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <f t="shared" si="0"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>102</v>
@@ -1668,7 +1652,7 @@
         <v>4</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="H38" s="1" t="s">
         <v>105</v>
@@ -1678,7 +1662,7 @@
     <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <f t="shared" si="0"/>
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>102</v>
@@ -1689,8 +1673,14 @@
       <c r="D39" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G39" s="1" t="s">
-        <v>28</v>
+      <c r="E39" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="G39" s="1">
+        <v>1</v>
       </c>
       <c r="H39" s="1" t="s">
         <v>105</v>
@@ -1700,7 +1690,7 @@
     <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <f t="shared" si="0"/>
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>102</v>
@@ -1711,8 +1701,14 @@
       <c r="D40" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G40" s="1" t="s">
-        <v>29</v>
+      <c r="E40" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="G40" s="1">
+        <v>2</v>
       </c>
       <c r="H40" s="1" t="s">
         <v>105</v>
@@ -1722,7 +1718,7 @@
     <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <f t="shared" si="0"/>
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>102</v>
@@ -1733,8 +1729,14 @@
       <c r="D41" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G41" s="1" t="s">
-        <v>30</v>
+      <c r="E41" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="G41" s="1">
+        <v>3</v>
       </c>
       <c r="H41" s="1" t="s">
         <v>105</v>
@@ -1744,7 +1746,7 @@
     <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <f t="shared" si="0"/>
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>102</v>
@@ -1756,13 +1758,13 @@
         <v>4</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="F42" s="1" t="s">
         <v>105</v>
       </c>
       <c r="G42" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H42" s="1" t="s">
         <v>105</v>
@@ -1772,7 +1774,7 @@
     <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
         <f t="shared" si="0"/>
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>102</v>
@@ -1784,13 +1786,13 @@
         <v>4</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="F43" s="1" t="s">
         <v>105</v>
       </c>
       <c r="G43" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H43" s="1" t="s">
         <v>105</v>
@@ -1800,7 +1802,7 @@
     <row r="44" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
         <f t="shared" si="0"/>
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>102</v>
@@ -1812,13 +1814,13 @@
         <v>4</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="F44" s="1" t="s">
         <v>105</v>
       </c>
       <c r="G44" s="1">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="H44" s="1" t="s">
         <v>105</v>
@@ -1828,7 +1830,7 @@
     <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
         <f t="shared" si="0"/>
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>102</v>
@@ -1839,24 +1841,27 @@
       <c r="D45" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E45" s="1" t="s">
-        <v>34</v>
+      <c r="E45" s="4" t="s">
+        <v>97</v>
       </c>
       <c r="F45" s="1" t="s">
         <v>105</v>
       </c>
       <c r="G45" s="1">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="H45" s="1" t="s">
         <v>105</v>
       </c>
       <c r="J45" s="1"/>
+      <c r="K45" s="6" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <f t="shared" si="0"/>
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>102</v>
@@ -1868,13 +1873,13 @@
         <v>4</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="F46" s="1" t="s">
         <v>105</v>
       </c>
       <c r="G46" s="1">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="H46" s="1" t="s">
         <v>105</v>
@@ -1884,7 +1889,7 @@
     <row r="47" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
         <f t="shared" si="0"/>
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>102</v>
@@ -1896,13 +1901,13 @@
         <v>4</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="F47" s="1" t="s">
         <v>105</v>
       </c>
       <c r="G47" s="1">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="H47" s="1" t="s">
         <v>105</v>
@@ -1912,7 +1917,7 @@
     <row r="48" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
         <f t="shared" si="0"/>
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>102</v>
@@ -1923,45 +1928,36 @@
       <c r="D48" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E48" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="F48" s="1" t="s">
-        <v>105</v>
-      </c>
       <c r="G48" s="1">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="H48" s="1" t="s">
         <v>105</v>
       </c>
       <c r="J48" s="1"/>
-      <c r="K48" s="6" t="s">
-        <v>96</v>
-      </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
         <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E49" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B49" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="D49" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E49" s="1" t="s">
-        <v>37</v>
-      </c>
       <c r="F49" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="G49" s="1">
-        <v>8</v>
+      <c r="G49" s="1" t="s">
+        <v>40</v>
       </c>
       <c r="H49" s="1" t="s">
         <v>105</v>
@@ -1971,7 +1967,7 @@
     <row r="50" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <f t="shared" si="0"/>
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>102</v>
@@ -1983,23 +1979,26 @@
         <v>4</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="F50" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="G50" s="1">
-        <v>9</v>
+      <c r="G50" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="H50" s="1" t="s">
         <v>105</v>
       </c>
       <c r="J50" s="1"/>
+      <c r="K50" s="6" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
         <f t="shared" si="0"/>
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>102</v>
@@ -2010,8 +2009,14 @@
       <c r="D51" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G51" s="1">
-        <v>0</v>
+      <c r="E51" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="G51" s="1" t="s">
+        <v>44</v>
       </c>
       <c r="H51" s="1" t="s">
         <v>105</v>
@@ -2021,7 +2026,7 @@
     <row r="52" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
         <f t="shared" si="0"/>
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>102</v>
@@ -2033,23 +2038,26 @@
         <v>4</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="F52" s="1" t="s">
         <v>105</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="H52" s="1" t="s">
         <v>105</v>
       </c>
       <c r="J52" s="1"/>
+      <c r="K52" s="6" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
         <f t="shared" si="0"/>
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>102</v>
@@ -2061,26 +2069,26 @@
         <v>4</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="F53" s="1" t="s">
         <v>105</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="H53" s="1" t="s">
         <v>105</v>
       </c>
       <c r="J53" s="1"/>
       <c r="K53" s="6" t="s">
-        <v>70</v>
+        <v>116</v>
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
         <f t="shared" si="0"/>
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>102</v>
@@ -2092,13 +2100,13 @@
         <v>4</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="F54" s="1" t="s">
         <v>105</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="H54" s="1" t="s">
         <v>105</v>
@@ -2108,7 +2116,7 @@
     <row r="55" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
         <f t="shared" si="0"/>
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>102</v>
@@ -2120,26 +2128,23 @@
         <v>4</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>45</v>
+        <v>73</v>
       </c>
       <c r="F55" s="1" t="s">
         <v>105</v>
       </c>
       <c r="G55" s="1" t="s">
-        <v>48</v>
+        <v>74</v>
       </c>
       <c r="H55" s="1" t="s">
         <v>105</v>
       </c>
       <c r="J55" s="1"/>
-      <c r="K55" s="6" t="s">
-        <v>115</v>
-      </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
         <f t="shared" si="0"/>
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>102</v>
@@ -2151,26 +2156,23 @@
         <v>4</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>47</v>
+        <v>75</v>
       </c>
       <c r="F56" s="1" t="s">
         <v>105</v>
       </c>
       <c r="G56" s="1" t="s">
-        <v>46</v>
+        <v>76</v>
       </c>
       <c r="H56" s="1" t="s">
         <v>105</v>
       </c>
       <c r="J56" s="1"/>
-      <c r="K56" s="6" t="s">
-        <v>116</v>
-      </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
         <f t="shared" si="0"/>
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>102</v>
@@ -2182,13 +2184,13 @@
         <v>4</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>49</v>
+        <v>77</v>
       </c>
       <c r="F57" s="1" t="s">
         <v>105</v>
       </c>
       <c r="G57" s="1" t="s">
-        <v>50</v>
+        <v>78</v>
       </c>
       <c r="H57" s="1" t="s">
         <v>105</v>
@@ -2198,7 +2200,7 @@
     <row r="58" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
         <f t="shared" si="0"/>
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>102</v>
@@ -2209,24 +2211,27 @@
       <c r="D58" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E58" s="1" t="s">
-        <v>73</v>
+      <c r="E58" s="4" t="s">
+        <v>80</v>
       </c>
       <c r="F58" s="1" t="s">
         <v>105</v>
       </c>
       <c r="G58" s="1" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="H58" s="1" t="s">
         <v>105</v>
       </c>
       <c r="J58" s="1"/>
+      <c r="K58" s="6" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
         <f t="shared" si="0"/>
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>102</v>
@@ -2237,24 +2242,27 @@
       <c r="D59" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E59" s="1" t="s">
-        <v>75</v>
+      <c r="E59" s="4" t="s">
+        <v>82</v>
       </c>
       <c r="F59" s="1" t="s">
         <v>105</v>
       </c>
       <c r="G59" s="1" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
       <c r="H59" s="1" t="s">
         <v>105</v>
       </c>
       <c r="J59" s="1"/>
+      <c r="K59" s="6" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
         <f t="shared" si="0"/>
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B60" s="1" t="s">
         <v>102</v>
@@ -2265,24 +2273,21 @@
       <c r="D60" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E60" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="F60" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="G60" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="H60" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="J60" s="1"/>
+      <c r="E60" s="4"/>
+      <c r="I60" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="J60" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="K60" s="6" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A61" s="1">
         <f t="shared" si="0"/>
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B61" s="1" t="s">
         <v>102</v>
@@ -2293,27 +2298,21 @@
       <c r="D61" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E61" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="F61" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="G61" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="H61" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="J61" s="1"/>
+      <c r="E61" s="4"/>
+      <c r="I61" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="J61" s="5" t="s">
+        <v>95</v>
+      </c>
       <c r="K61" s="6" t="s">
-        <v>81</v>
+        <v>92</v>
       </c>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
         <f t="shared" si="0"/>
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>102</v>
@@ -2324,27 +2323,21 @@
       <c r="D62" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E62" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="F62" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="G62" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="H62" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="J62" s="1"/>
+      <c r="E62" s="4"/>
+      <c r="I62" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="J62" s="5" t="s">
+        <v>95</v>
+      </c>
       <c r="K62" s="6" t="s">
-        <v>84</v>
+        <v>93</v>
       </c>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
         <f t="shared" si="0"/>
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>102</v>
@@ -2357,106 +2350,94 @@
       </c>
       <c r="E63" s="4"/>
       <c r="I63" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="J63" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="J63" s="5" t="s">
         <v>95</v>
       </c>
       <c r="K63" s="6" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A64" s="1">
         <f t="shared" si="0"/>
+        <v>55</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I64" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B64" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="C64" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="D64" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E64" s="4"/>
-      <c r="I64" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="J64" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="K64" s="6" t="s">
-        <v>92</v>
+      <c r="J64" s="1" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A65" s="1">
         <f t="shared" si="0"/>
+        <v>56</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I65" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B65" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="C65" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="D65" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E65" s="4"/>
-      <c r="I65" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="J65" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="K65" s="6" t="s">
-        <v>93</v>
+      <c r="J65" s="1" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A66" s="1">
         <f t="shared" si="0"/>
+        <v>57</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I66" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B66" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="C66" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="D66" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E66" s="4"/>
-      <c r="I66" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="J66" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="K66" s="6" t="s">
-        <v>94</v>
+      <c r="J66" s="1" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A67" s="1">
         <f t="shared" si="0"/>
+        <v>58</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I67" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="B67" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="C67" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="D67" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="I67" s="1" t="s">
-        <v>54</v>
       </c>
       <c r="J67" s="1" t="s">
         <v>53</v>
@@ -2465,7 +2446,7 @@
     <row r="68" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A68" s="1">
         <f t="shared" si="0"/>
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>102</v>
@@ -2477,7 +2458,7 @@
         <v>4</v>
       </c>
       <c r="I68" s="1" t="s">
-        <v>55</v>
+        <v>71</v>
       </c>
       <c r="J68" s="1" t="s">
         <v>53</v>
@@ -2486,7 +2467,7 @@
     <row r="69" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A69" s="1">
         <f t="shared" si="0"/>
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B69" s="1" t="s">
         <v>102</v>
@@ -2498,16 +2479,17 @@
         <v>4</v>
       </c>
       <c r="I69" s="1" t="s">
-        <v>56</v>
+        <v>86</v>
       </c>
       <c r="J69" s="1" t="s">
         <v>53</v>
       </c>
+      <c r="K69" s="7"/>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A70" s="1">
         <f t="shared" si="0"/>
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B70" s="1" t="s">
         <v>102</v>
@@ -2519,7 +2501,7 @@
         <v>4</v>
       </c>
       <c r="I70" s="1" t="s">
-        <v>57</v>
+        <v>110</v>
       </c>
       <c r="J70" s="1" t="s">
         <v>53</v>
@@ -2528,28 +2510,35 @@
     <row r="71" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A71" s="1">
         <f t="shared" si="0"/>
+        <v>62</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E71" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B71" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="C71" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="D71" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="I71" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="J71" s="1" t="s">
+      <c r="F71" s="1" t="s">
         <v>53</v>
       </c>
+      <c r="G71" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="H71" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="J71" s="1"/>
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A72" s="1">
         <f t="shared" si="0"/>
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B72" s="1" t="s">
         <v>102</v>
@@ -2560,39 +2549,52 @@
       <c r="D72" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="I72" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="J72" s="1" t="s">
+      <c r="E72" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F72" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="K72" s="7"/>
+      <c r="G72" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H72" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="J72" s="1"/>
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A73" s="1">
         <f t="shared" si="0"/>
+        <v>64</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E73" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F73" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G73" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B73" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="C73" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="D73" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="I73" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="J73" s="1" t="s">
+      <c r="H73" s="1" t="s">
         <v>53</v>
       </c>
+      <c r="J73" s="1"/>
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A74" s="1">
         <f t="shared" si="0"/>
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B74" s="1" t="s">
         <v>102</v>
@@ -2604,13 +2606,13 @@
         <v>4</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>61</v>
+        <v>72</v>
       </c>
       <c r="F74" s="1" t="s">
         <v>53</v>
       </c>
       <c r="G74" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H74" s="1" t="s">
         <v>53</v>
@@ -2620,7 +2622,7 @@
     <row r="75" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A75" s="1">
         <f t="shared" si="0"/>
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B75" s="1" t="s">
         <v>102</v>
@@ -2632,23 +2634,24 @@
         <v>4</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>64</v>
+        <v>108</v>
       </c>
       <c r="F75" s="1" t="s">
         <v>53</v>
       </c>
       <c r="G75" s="1" t="s">
-        <v>65</v>
+        <v>109</v>
       </c>
       <c r="H75" s="1" t="s">
         <v>53</v>
       </c>
       <c r="J75" s="1"/>
+      <c r="K75" s="7"/>
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A76" s="1">
-        <f t="shared" si="0"/>
-        <v>66</v>
+        <f t="shared" ref="A76:A81" si="1">A75+1</f>
+        <v>67</v>
       </c>
       <c r="B76" s="1" t="s">
         <v>102</v>
@@ -2657,26 +2660,22 @@
         <v>112</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E76" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="I76" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F76" s="1" t="s">
+      <c r="J76" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="G76" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="H76" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="J76" s="1"/>
+      <c r="K76" s="6" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A77" s="1">
-        <f t="shared" si="0"/>
-        <v>67</v>
+        <f t="shared" si="1"/>
+        <v>68</v>
       </c>
       <c r="B77" s="1" t="s">
         <v>102</v>
@@ -2685,26 +2684,22 @@
         <v>112</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E77" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="F77" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="I77" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="J77" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="G77" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="H77" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="J77" s="1"/>
+      <c r="K77" s="6" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A78" s="1">
-        <f t="shared" ref="A78:A84" si="1">A77+1</f>
-        <v>68</v>
+        <f t="shared" si="1"/>
+        <v>69</v>
       </c>
       <c r="B78" s="1" t="s">
         <v>102</v>
@@ -2713,27 +2708,19 @@
         <v>112</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E78" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="F78" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="I78" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="J78" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="G78" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="H78" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="J78" s="1"/>
-      <c r="K78" s="7"/>
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A79" s="1">
         <f t="shared" si="1"/>
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B79" s="1" t="s">
         <v>102</v>
@@ -2745,145 +2732,109 @@
         <v>51</v>
       </c>
       <c r="I79" s="1" t="s">
-        <v>52</v>
+        <v>71</v>
       </c>
       <c r="J79" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="K79" s="6" t="s">
-        <v>69</v>
-      </c>
+      <c r="K79" s="7"/>
     </row>
     <row r="80" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A80" s="1">
         <f t="shared" si="1"/>
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B80" s="1" t="s">
         <v>102</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="I80" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="J80" s="1" t="s">
-        <v>53</v>
-      </c>
+        <v>103</v>
+      </c>
+      <c r="E80"/>
+      <c r="F80"/>
+      <c r="G80"/>
+      <c r="H80"/>
+      <c r="I80"/>
       <c r="K80" s="6" t="s">
-        <v>68</v>
+        <v>104</v>
       </c>
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A81" s="1">
         <f t="shared" si="1"/>
-        <v>71</v>
-      </c>
-      <c r="B81" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="C81" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="D81" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="I81" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="J81" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B81" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="C81" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="D81" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E81" s="8"/>
+      <c r="F81" s="8"/>
+      <c r="G81" s="8"/>
+      <c r="H81" s="8"/>
+      <c r="I81" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="J81" s="9" t="s">
         <v>53</v>
       </c>
+      <c r="K81" s="10" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A82" s="1">
-        <f t="shared" si="1"/>
-        <v>72</v>
-      </c>
-      <c r="B82" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="C82" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="D82" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="I82" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="J82" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="K82" s="7"/>
+      <c r="A82" s="5"/>
+      <c r="B82" s="5"/>
+      <c r="C82" s="5"/>
+      <c r="D82" s="5"/>
+      <c r="E82" s="8"/>
+      <c r="F82" s="8"/>
+      <c r="G82" s="8"/>
+      <c r="H82" s="8"/>
+      <c r="I82" s="5"/>
+      <c r="J82" s="9"/>
+      <c r="K82" s="10"/>
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A83" s="1">
-        <f t="shared" si="1"/>
-        <v>73</v>
-      </c>
-      <c r="B83" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="C83" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="D83" s="1" t="s">
-        <v>103</v>
-      </c>
+      <c r="A83"/>
+      <c r="B83"/>
+      <c r="C83"/>
+      <c r="D83"/>
       <c r="E83"/>
       <c r="F83"/>
       <c r="G83"/>
       <c r="H83"/>
       <c r="I83"/>
-      <c r="K83" s="6" t="s">
-        <v>104</v>
-      </c>
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A84" s="1">
-        <f t="shared" si="1"/>
-        <v>74</v>
-      </c>
-      <c r="B84" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="C84" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="D84" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="E84" s="8"/>
-      <c r="F84" s="8"/>
-      <c r="G84" s="8"/>
-      <c r="H84" s="8"/>
-      <c r="I84" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="J84" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="K84" s="10" t="s">
-        <v>114</v>
-      </c>
+      <c r="A84"/>
+      <c r="B84"/>
+      <c r="C84"/>
+      <c r="D84"/>
+      <c r="E84"/>
+      <c r="F84"/>
+      <c r="G84"/>
+      <c r="H84"/>
+      <c r="I84"/>
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A85" s="5"/>
-      <c r="B85" s="5"/>
-      <c r="C85" s="5"/>
-      <c r="D85" s="5"/>
-      <c r="E85" s="8"/>
-      <c r="F85" s="8"/>
-      <c r="G85" s="8"/>
-      <c r="H85" s="8"/>
-      <c r="I85" s="5"/>
-      <c r="J85" s="9"/>
-      <c r="K85" s="10"/>
+      <c r="A85"/>
+      <c r="B85"/>
+      <c r="C85"/>
+      <c r="D85"/>
+      <c r="E85"/>
+      <c r="F85"/>
+      <c r="G85"/>
+      <c r="H85"/>
+      <c r="I85"/>
     </row>
     <row r="86" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A86"/>
@@ -2895,39 +2846,6 @@
       <c r="G86"/>
       <c r="H86"/>
       <c r="I86"/>
-    </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A87"/>
-      <c r="B87"/>
-      <c r="C87"/>
-      <c r="D87"/>
-      <c r="E87"/>
-      <c r="F87"/>
-      <c r="G87"/>
-      <c r="H87"/>
-      <c r="I87"/>
-    </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A88"/>
-      <c r="B88"/>
-      <c r="C88"/>
-      <c r="D88"/>
-      <c r="E88"/>
-      <c r="F88"/>
-      <c r="G88"/>
-      <c r="H88"/>
-      <c r="I88"/>
-    </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A89"/>
-      <c r="B89"/>
-      <c r="C89"/>
-      <c r="D89"/>
-      <c r="E89"/>
-      <c r="F89"/>
-      <c r="G89"/>
-      <c r="H89"/>
-      <c r="I89"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
Fix number row sizes in keycap spec
</commit_message>
<xml_diff>
--- a/hardware/keyboard-classic/classic-ascii-keycaps.xlsx
+++ b/hardware/keyboard-classic/classic-ascii-keycaps.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dave/vsrc/unified_retro_keyboard/hardware/keyboard-classic/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/User/dave/vsrc/unified_retro_keyboard/hardware/keyboard-classic/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB34F5F8-E37A-6E4D-9902-102EE7F8EC93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B95A577-77E0-3546-B390-F44C98F5F5AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19640" yWindow="5360" windowWidth="41160" windowHeight="30100" xr2:uid="{5947D8F6-B0FF-824B-90A6-066CA128251B}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="115">
   <si>
     <t>Size</t>
   </si>
@@ -155,37 +155,19 @@
     <t>*</t>
   </si>
   <si>
-    <t>:</t>
-  </si>
-  <si>
     <t>=</t>
   </si>
   <si>
-    <t>-</t>
-  </si>
-  <si>
     <t>+</t>
   </si>
   <si>
-    <t>;</t>
-  </si>
-  <si>
     <t>&lt; </t>
   </si>
   <si>
-    <t>.</t>
-  </si>
-  <si>
     <t>&gt; </t>
   </si>
   <si>
-    <t>,</t>
-  </si>
-  <si>
     <t>?</t>
-  </si>
-  <si>
-    <t>/</t>
   </si>
   <si>
     <t>1.5u</t>
@@ -260,15 +242,9 @@
     <t>{</t>
   </si>
   <si>
-    <t>[</t>
-  </si>
-  <si>
     <t>}</t>
   </si>
   <si>
-    <t>]</t>
-  </si>
-  <si>
     <t>~</t>
   </si>
   <si>
@@ -287,9 +263,6 @@
     <t>|</t>
   </si>
   <si>
-    <t>\</t>
-  </si>
-  <si>
     <t>vertical bar and backslash</t>
   </si>
   <si>
@@ -405,6 +378,9 @@
   </si>
   <si>
     <t>Classic Keycap set</t>
+  </si>
+  <si>
+    <t>.150"</t>
   </si>
 </sst>
 </file>
@@ -447,7 +423,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -467,17 +443,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -863,8 +833,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D76B701B-B3BE-9240-9526-A5AC01D01246}">
   <dimension ref="A1:K86"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="161" zoomScaleNormal="161" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="161" zoomScaleNormal="161" workbookViewId="0">
+      <selection activeCell="G39" sqref="G39:G59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -882,96 +852,91 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A1" s="14" t="s">
-        <v>122</v>
-      </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="15" t="s">
-        <v>99</v>
-      </c>
-      <c r="F1" s="15"/>
-      <c r="G1" s="16">
+      <c r="A1" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="F1" s="13"/>
+      <c r="G1" s="14">
         <v>44529</v>
       </c>
-      <c r="H1" s="14"/>
+      <c r="H1" s="12"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A2" s="11"/>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="11"/>
-      <c r="K2" s="11"/>
+      <c r="A2" s="6"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="6"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A3" s="11" t="s">
-        <v>121</v>
-      </c>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="13"/>
-      <c r="H3" s="11"/>
-      <c r="K3" s="11"/>
+      <c r="A3" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="6"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4" s="11" t="s">
-        <v>119</v>
-      </c>
-      <c r="B4" s="11"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="11"/>
-      <c r="K4" s="11"/>
+      <c r="A4" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="6"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A5" s="11" t="s">
-        <v>117</v>
-      </c>
-      <c r="B5" s="11"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="13"/>
-      <c r="H5" s="11"/>
-      <c r="K5" s="11"/>
+      <c r="A5" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="6"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A6" s="11"/>
-      <c r="B6" s="11"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="13"/>
-      <c r="H6" s="11"/>
-      <c r="K6" s="11"/>
+      <c r="A6" s="6"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="6"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>0</v>
@@ -980,22 +945,22 @@
         <v>1</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>2</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>3</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="K9" s="6" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
@@ -1003,10 +968,10 @@
         <v>1</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>4</v>
@@ -1015,7 +980,7 @@
         <v>5</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="J10" s="1"/>
     </row>
@@ -1025,10 +990,10 @@
         <v>2</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>4</v>
@@ -1037,7 +1002,7 @@
         <v>6</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="J11" s="1"/>
     </row>
@@ -1047,10 +1012,10 @@
         <v>3</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>4</v>
@@ -1059,7 +1024,7 @@
         <v>7</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="J12" s="1"/>
     </row>
@@ -1069,10 +1034,10 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>4</v>
@@ -1081,7 +1046,7 @@
         <v>8</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="J13" s="1"/>
     </row>
@@ -1091,10 +1056,10 @@
         <v>5</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>4</v>
@@ -1103,7 +1068,7 @@
         <v>9</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="J14" s="1"/>
     </row>
@@ -1113,10 +1078,10 @@
         <v>6</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>4</v>
@@ -1125,11 +1090,11 @@
         <v>10</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="J15" s="1"/>
       <c r="K15" s="6" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
@@ -1138,25 +1103,25 @@
         <v>7</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>4</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="G16" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="J16" s="1"/>
     </row>
@@ -1166,10 +1131,10 @@
         <v>8</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>4</v>
@@ -1178,7 +1143,7 @@
         <v>11</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="J17" s="1"/>
     </row>
@@ -1188,10 +1153,10 @@
         <v>9</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>4</v>
@@ -1200,7 +1165,7 @@
         <v>12</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="J18" s="1"/>
     </row>
@@ -1210,10 +1175,10 @@
         <v>10</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>4</v>
@@ -1222,7 +1187,7 @@
         <v>13</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="J19" s="1"/>
     </row>
@@ -1232,10 +1197,10 @@
         <v>11</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>4</v>
@@ -1244,11 +1209,11 @@
         <v>14</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="J20" s="1"/>
       <c r="K20" s="6" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
@@ -1257,10 +1222,10 @@
         <v>12</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>4</v>
@@ -1269,7 +1234,7 @@
         <v>15</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="J21" s="1"/>
     </row>
@@ -1279,10 +1244,10 @@
         <v>13</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>4</v>
@@ -1291,7 +1256,7 @@
         <v>16</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="J22" s="1"/>
     </row>
@@ -1301,10 +1266,10 @@
         <v>14</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>4</v>
@@ -1313,7 +1278,7 @@
         <v>17</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="J23" s="1"/>
     </row>
@@ -1323,10 +1288,10 @@
         <v>15</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>4</v>
@@ -1335,7 +1300,7 @@
         <v>18</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="J24" s="1"/>
     </row>
@@ -1345,25 +1310,25 @@
         <v>16</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>4</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="G25" s="1" t="s">
         <v>18</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="J25" s="1"/>
     </row>
@@ -1373,10 +1338,10 @@
         <v>17</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>4</v>
@@ -1385,7 +1350,7 @@
         <v>19</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="J26" s="1"/>
     </row>
@@ -1395,10 +1360,10 @@
         <v>18</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>4</v>
@@ -1407,7 +1372,7 @@
         <v>20</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="J27" s="1"/>
     </row>
@@ -1417,25 +1382,25 @@
         <v>19</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>4</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="G28" s="1" t="s">
         <v>20</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="J28" s="1"/>
     </row>
@@ -1445,10 +1410,10 @@
         <v>20</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>4</v>
@@ -1457,7 +1422,7 @@
         <v>21</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="J29" s="1"/>
     </row>
@@ -1467,10 +1432,10 @@
         <v>21</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>4</v>
@@ -1479,7 +1444,7 @@
         <v>22</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="J30" s="1"/>
     </row>
@@ -1489,10 +1454,10 @@
         <v>22</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>4</v>
@@ -1501,7 +1466,7 @@
         <v>23</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="J31" s="1"/>
     </row>
@@ -1511,10 +1476,10 @@
         <v>23</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>4</v>
@@ -1523,7 +1488,7 @@
         <v>24</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="J32" s="1"/>
     </row>
@@ -1533,10 +1498,10 @@
         <v>24</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>4</v>
@@ -1545,7 +1510,7 @@
         <v>25</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="J33" s="1"/>
     </row>
@@ -1555,10 +1520,10 @@
         <v>25</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>4</v>
@@ -1567,7 +1532,7 @@
         <v>26</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="J34" s="1"/>
     </row>
@@ -1577,10 +1542,10 @@
         <v>26</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>4</v>
@@ -1589,7 +1554,7 @@
         <v>27</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="J35" s="1"/>
     </row>
@@ -1599,10 +1564,10 @@
         <v>27</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>4</v>
@@ -1611,7 +1576,7 @@
         <v>28</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="J36" s="1"/>
     </row>
@@ -1621,10 +1586,10 @@
         <v>28</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>4</v>
@@ -1633,7 +1598,7 @@
         <v>29</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="J37" s="1"/>
     </row>
@@ -1643,10 +1608,10 @@
         <v>29</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>4</v>
@@ -1655,7 +1620,7 @@
         <v>30</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="J38" s="1"/>
     </row>
@@ -1665,10 +1630,10 @@
         <v>30</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>4</v>
@@ -1677,13 +1642,13 @@
         <v>31</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="G39" s="1">
-        <v>1</v>
+        <v>114</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>114</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="J39" s="1"/>
     </row>
@@ -1693,10 +1658,10 @@
         <v>31</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>4</v>
@@ -1705,13 +1670,13 @@
         <v>32</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="G40" s="1">
-        <v>2</v>
+        <v>114</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>114</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="J40" s="1"/>
     </row>
@@ -1721,10 +1686,10 @@
         <v>32</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>4</v>
@@ -1733,13 +1698,13 @@
         <v>33</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="G41" s="1">
-        <v>3</v>
+        <v>114</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>114</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="J41" s="1"/>
     </row>
@@ -1749,10 +1714,10 @@
         <v>33</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>4</v>
@@ -1761,13 +1726,13 @@
         <v>34</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="G42" s="1">
-        <v>4</v>
+        <v>114</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>114</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="J42" s="1"/>
     </row>
@@ -1777,10 +1742,10 @@
         <v>34</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>4</v>
@@ -1789,13 +1754,13 @@
         <v>35</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="G43" s="1">
-        <v>5</v>
+        <v>114</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>114</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="J43" s="1"/>
     </row>
@@ -1805,10 +1770,10 @@
         <v>35</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>4</v>
@@ -1817,13 +1782,13 @@
         <v>36</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="G44" s="1">
-        <v>6</v>
+        <v>114</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>114</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="J44" s="1"/>
     </row>
@@ -1833,29 +1798,29 @@
         <v>36</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>4</v>
       </c>
       <c r="E45" s="4" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="G45" s="1">
-        <v>7</v>
+        <v>114</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>114</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="J45" s="1"/>
       <c r="K45" s="6" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.2">
@@ -1864,10 +1829,10 @@
         <v>37</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>4</v>
@@ -1876,13 +1841,13 @@
         <v>37</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="G46" s="1">
-        <v>8</v>
+        <v>114</v>
+      </c>
+      <c r="G46" s="1" t="s">
+        <v>114</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="J46" s="1"/>
     </row>
@@ -1892,10 +1857,10 @@
         <v>38</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>4</v>
@@ -1904,13 +1869,13 @@
         <v>38</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="G47" s="1">
-        <v>9</v>
+        <v>114</v>
+      </c>
+      <c r="G47" s="1" t="s">
+        <v>114</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="J47" s="1"/>
     </row>
@@ -1920,19 +1885,19 @@
         <v>39</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G48" s="1">
-        <v>0</v>
+      <c r="G48" s="1" t="s">
+        <v>114</v>
       </c>
       <c r="H48" s="1" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="J48" s="1"/>
     </row>
@@ -1942,10 +1907,10 @@
         <v>40</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>4</v>
@@ -1954,13 +1919,13 @@
         <v>39</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>40</v>
+        <v>114</v>
       </c>
       <c r="H49" s="1" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="J49" s="1"/>
     </row>
@@ -1970,29 +1935,29 @@
         <v>41</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>4</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>42</v>
+        <v>114</v>
       </c>
       <c r="H50" s="1" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="J50" s="1"/>
       <c r="K50" s="6" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.2">
@@ -2001,25 +1966,25 @@
         <v>42</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>4</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>44</v>
+        <v>114</v>
       </c>
       <c r="H51" s="1" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="J51" s="1"/>
     </row>
@@ -2029,29 +1994,29 @@
         <v>43</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>4</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>48</v>
+        <v>114</v>
       </c>
       <c r="H52" s="1" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="J52" s="1"/>
       <c r="K52" s="6" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.2">
@@ -2060,29 +2025,29 @@
         <v>44</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>4</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>46</v>
+        <v>114</v>
       </c>
       <c r="H53" s="1" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="J53" s="1"/>
       <c r="K53" s="6" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.2">
@@ -2091,25 +2056,25 @@
         <v>45</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>4</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>50</v>
+        <v>114</v>
       </c>
       <c r="H54" s="1" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="J54" s="1"/>
     </row>
@@ -2119,25 +2084,25 @@
         <v>46</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>4</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c r="G55" s="1" t="s">
-        <v>74</v>
+        <v>114</v>
       </c>
       <c r="H55" s="1" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="J55" s="1"/>
     </row>
@@ -2147,25 +2112,25 @@
         <v>47</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>4</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c r="G56" s="1" t="s">
-        <v>76</v>
+        <v>114</v>
       </c>
       <c r="H56" s="1" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="J56" s="1"/>
     </row>
@@ -2175,25 +2140,25 @@
         <v>48</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="D57" s="1" t="s">
         <v>4</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c r="G57" s="1" t="s">
-        <v>78</v>
+        <v>114</v>
       </c>
       <c r="H57" s="1" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="J57" s="1"/>
     </row>
@@ -2203,29 +2168,29 @@
         <v>49</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>4</v>
       </c>
       <c r="E58" s="4" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c r="G58" s="1" t="s">
-        <v>79</v>
+        <v>114</v>
       </c>
       <c r="H58" s="1" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="J58" s="1"/>
       <c r="K58" s="6" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.2">
@@ -2234,29 +2199,29 @@
         <v>50</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>4</v>
       </c>
       <c r="E59" s="4" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c r="G59" s="1" t="s">
-        <v>83</v>
+        <v>114</v>
       </c>
       <c r="H59" s="1" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="J59" s="1"/>
       <c r="K59" s="6" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.2">
@@ -2265,23 +2230,23 @@
         <v>51</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>4</v>
       </c>
       <c r="E60" s="4"/>
       <c r="I60" s="1" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="J60" s="1" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="K60" s="6" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.2">
@@ -2290,23 +2255,23 @@
         <v>52</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="D61" s="1" t="s">
         <v>4</v>
       </c>
       <c r="E61" s="4"/>
       <c r="I61" s="1" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="J61" s="5" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="K61" s="6" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.2">
@@ -2315,23 +2280,23 @@
         <v>53</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>4</v>
       </c>
       <c r="E62" s="4"/>
       <c r="I62" s="1" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="J62" s="5" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="K62" s="6" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.2">
@@ -2340,23 +2305,23 @@
         <v>54</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="D63" s="1" t="s">
         <v>4</v>
       </c>
       <c r="E63" s="4"/>
       <c r="I63" s="1" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="J63" s="5" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="K63" s="6" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.2">
@@ -2365,19 +2330,19 @@
         <v>55</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="D64" s="1" t="s">
         <v>4</v>
       </c>
       <c r="I64" s="1" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="J64" s="1" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.2">
@@ -2386,19 +2351,19 @@
         <v>56</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="D65" s="1" t="s">
         <v>4</v>
       </c>
       <c r="I65" s="1" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="J65" s="1" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.2">
@@ -2407,19 +2372,19 @@
         <v>57</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="D66" s="1" t="s">
         <v>4</v>
       </c>
       <c r="I66" s="1" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="J66" s="1" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.2">
@@ -2428,19 +2393,19 @@
         <v>58</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="D67" s="1" t="s">
         <v>4</v>
       </c>
       <c r="I67" s="1" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="J67" s="1" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.2">
@@ -2449,19 +2414,19 @@
         <v>59</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="D68" s="1" t="s">
         <v>4</v>
       </c>
       <c r="I68" s="1" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="J68" s="1" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.2">
@@ -2470,21 +2435,20 @@
         <v>60</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="D69" s="1" t="s">
         <v>4</v>
       </c>
       <c r="I69" s="1" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="J69" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="K69" s="7"/>
+        <v>47</v>
+      </c>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A70" s="1">
@@ -2492,19 +2456,19 @@
         <v>61</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="D70" s="1" t="s">
         <v>4</v>
       </c>
       <c r="I70" s="1" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="J70" s="1" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.2">
@@ -2513,25 +2477,25 @@
         <v>62</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="D71" s="1" t="s">
         <v>4</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="G71" s="1" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="H71" s="1" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="J71" s="1"/>
     </row>
@@ -2541,25 +2505,25 @@
         <v>63</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="D72" s="1" t="s">
         <v>4</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="G72" s="1" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="H72" s="1" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="J72" s="1"/>
     </row>
@@ -2569,25 +2533,25 @@
         <v>64</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="D73" s="1" t="s">
         <v>4</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="G73" s="1" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="H73" s="1" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="J73" s="1"/>
     </row>
@@ -2597,25 +2561,25 @@
         <v>65</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="D74" s="1" t="s">
         <v>4</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="G74" s="1" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="H74" s="1" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="J74" s="1"/>
     </row>
@@ -2625,28 +2589,27 @@
         <v>66</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="D75" s="1" t="s">
         <v>4</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="G75" s="1" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="H75" s="1" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="J75" s="1"/>
-      <c r="K75" s="7"/>
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A76" s="1">
@@ -2654,22 +2617,22 @@
         <v>67</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="I76" s="1" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="J76" s="1" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="K76" s="6" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.2">
@@ -2678,22 +2641,22 @@
         <v>68</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="I77" s="1" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="J77" s="1" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="K77" s="6" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.2">
@@ -2702,19 +2665,19 @@
         <v>69</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="I78" s="1" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="J78" s="1" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.2">
@@ -2723,21 +2686,20 @@
         <v>70</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="I79" s="1" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="J79" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="K79" s="7"/>
+        <v>47</v>
+      </c>
     </row>
     <row r="80" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A80" s="1">
@@ -2745,13 +2707,13 @@
         <v>71</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="E80"/>
       <c r="F80"/>
@@ -2759,7 +2721,7 @@
       <c r="H80"/>
       <c r="I80"/>
       <c r="K80" s="6" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.2">
@@ -2768,26 +2730,26 @@
         <v>72</v>
       </c>
       <c r="B81" s="5" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="C81" s="5" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="D81" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E81" s="8"/>
-      <c r="F81" s="8"/>
-      <c r="G81" s="8"/>
-      <c r="H81" s="8"/>
+      <c r="E81" s="7"/>
+      <c r="F81" s="7"/>
+      <c r="G81" s="7"/>
+      <c r="H81" s="7"/>
       <c r="I81" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="J81" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="K81" s="10" t="s">
-        <v>114</v>
+        <v>98</v>
+      </c>
+      <c r="J81" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="K81" s="9" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.2">
@@ -2795,13 +2757,13 @@
       <c r="B82" s="5"/>
       <c r="C82" s="5"/>
       <c r="D82" s="5"/>
-      <c r="E82" s="8"/>
-      <c r="F82" s="8"/>
-      <c r="G82" s="8"/>
-      <c r="H82" s="8"/>
+      <c r="E82" s="7"/>
+      <c r="F82" s="7"/>
+      <c r="G82" s="7"/>
+      <c r="H82" s="7"/>
       <c r="I82" s="5"/>
-      <c r="J82" s="9"/>
-      <c r="K82" s="10"/>
+      <c r="J82" s="8"/>
+      <c r="K82" s="9"/>
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A83"/>

</xml_diff>